<commit_message>
cambio de ambiente de pruebas, ejercicio parte uno finalizado
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Test.xlsx
+++ b/src/test/resources/data/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>dresses</t>
   </si>
@@ -42,23 +42,22 @@
     <t>shot</t>
   </si>
   <si>
-    <t>pass1</t>
-  </si>
-  <si>
-    <t>Nazareno</t>
-  </si>
-  <si>
-    <t>registrado</t>
-  </si>
-  <si>
-    <t>activo</t>
+    <t>user@phptravels.com</t>
+  </si>
+  <si>
+    <t>demouser</t>
+  </si>
+  <si>
+    <t>demoadmin</t>
+  </si>
+  <si>
+    <t>admin@phptravels.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,29 +403,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -447,7 +443,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,33 +485,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
código refactorizado de ejercicio apache poi
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Test.xlsx
+++ b/src/test/resources/data/Test.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="3435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Credenciales" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>dresses</t>
   </si>
@@ -403,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -412,17 +412,20 @@
     <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -487,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
borré la clase de Register_Test.java que correspondía a otro ejercicio
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Test.xlsx
+++ b/src/test/resources/data/Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>dresses</t>
   </si>
@@ -52,12 +52,19 @@
   </si>
   <si>
     <t>admin@phptravels.com</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>disponible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -409,7 +416,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -443,7 +450,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -485,7 +492,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -493,10 +500,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -506,6 +513,9 @@
       <c r="B1" t="s">
         <v>9</v>
       </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -513,6 +523,9 @@
       </c>
       <c r="B2" t="s">
         <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>